<commit_message>
Added decimal to percents. added IPS AIP calculations to script
</commit_message>
<xml_diff>
--- a/outputs/Voluntary Turnover Rate Monthly 2025-01-01 to 2025-02-28.xlsx
+++ b/outputs/Voluntary Turnover Rate Monthly 2025-01-01 to 2025-02-28.xlsx
@@ -1108,20 +1108,20 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="14">
-    <numFmt numFmtId="165" formatCode="0%"/>
-    <numFmt numFmtId="166" formatCode="0%"/>
-    <numFmt numFmtId="167" formatCode="0%"/>
-    <numFmt numFmtId="168" formatCode="0%"/>
-    <numFmt numFmtId="169" formatCode="0%"/>
-    <numFmt numFmtId="170" formatCode="0%"/>
-    <numFmt numFmtId="171" formatCode="0%"/>
-    <numFmt numFmtId="172" formatCode="0%"/>
-    <numFmt numFmtId="173" formatCode="0%"/>
-    <numFmt numFmtId="174" formatCode="0%"/>
-    <numFmt numFmtId="175" formatCode="0%"/>
-    <numFmt numFmtId="176" formatCode="0%"/>
-    <numFmt numFmtId="177" formatCode="0%"/>
-    <numFmt numFmtId="178" formatCode="0%"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
+    <numFmt numFmtId="167" formatCode="0.0%"/>
+    <numFmt numFmtId="168" formatCode="0.0%"/>
+    <numFmt numFmtId="169" formatCode="0.0%"/>
+    <numFmt numFmtId="170" formatCode="0.0%"/>
+    <numFmt numFmtId="171" formatCode="0.0%"/>
+    <numFmt numFmtId="172" formatCode="0.0%"/>
+    <numFmt numFmtId="173" formatCode="0.0%"/>
+    <numFmt numFmtId="174" formatCode="0.0%"/>
+    <numFmt numFmtId="175" formatCode="0.0%"/>
+    <numFmt numFmtId="176" formatCode="0.0%"/>
+    <numFmt numFmtId="177" formatCode="0.0%"/>
+    <numFmt numFmtId="178" formatCode="0.0%"/>
   </numFmts>
   <fonts count="2">
     <font>

</xml_diff>